<commit_message>
Add Dynare model for Ramsey transition analysis
Introduces ramsey_stationary_transition.mod to study transition dynamics in a nonstationary Ramsey model using Dynare. The model analyzes the effects of a change in the discount factor (beta) from 0.95 to 0.99, simulating the transition between steady states. Also updates readme.xlsx.
</commit_message>
<xml_diff>
--- a/readme.xlsx
+++ b/readme.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u477193\personal backup\github\DSGE_mod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E582BC08-AC9C-4223-AB21-F4F33C469D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB66E88-0608-4C27-BA04-7EF709E86922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t>Solow Model</t>
   </si>
@@ -123,17 +134,47 @@
     <t>√</t>
   </si>
   <si>
-    <t>Ramsey_Cass_Koopmans</t>
-  </si>
-  <si>
     <t>Folder</t>
+  </si>
+  <si>
+    <t>Paper / Model</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Publication Year</t>
+  </si>
+  <si>
+    <t>Ramsey_SS_transition</t>
+  </si>
+  <si>
+    <t>Ramsey_BGP</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Studies the transition dynamics of a simple Ramsey model from its old steady state to its steady state when there is a permanent unexpected change (in the code, β changes from 0.95 to 0.99)</t>
+  </si>
+  <si>
+    <t>Studies the transition dynamics of a simple Ramsey economy  to its balanced growth path (BGP). The RCK model is solved here in aggregate, i.e. non-detrended form along its balanced growth path. For that purpose, trending labor-augmenting technology (A) and population processes (L) are defined.</t>
+  </si>
+  <si>
+    <t>β is the `varexo` (exogenous variable).  Use `initval` block with old steady state and β=0.95; Use `endval` block with new steady state and β=0.99. No need to use `shock` block because Dynare assume β =0.99 since the first period.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A and L are `varexo`. In addition to `initval` block and `endval` block, we still need `shock` block to specify the path of A and L (the value of A and L in each period except the last period).	</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,25 +188,21 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -180,15 +217,53 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,263 +544,381 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="85.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="6" max="6" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="8.88671875" style="10"/>
+    <col min="3" max="3" width="54.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16" style="15" customWidth="1"/>
+    <col min="5" max="5" width="20.88671875" style="8" customWidth="1"/>
+    <col min="6" max="6" width="15" style="8" customWidth="1"/>
+    <col min="7" max="7" width="67.109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="81.5546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F1" t="s">
+      <c r="C1" s="6" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="D1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="10"/>
+      <c r="F2" s="8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5">
+    <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="10">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="14"/>
+      <c r="E3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="G3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="10">
+        <v>3</v>
+      </c>
+      <c r="B4" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="C4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="14"/>
+      <c r="E4" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="10">
+        <v>4</v>
+      </c>
+      <c r="B5" s="14"/>
+      <c r="C5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="D5" s="14"/>
+      <c r="F5" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="10">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" s="10"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="10">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="D7" s="10"/>
+    </row>
+    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="10">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="10">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="10">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D9" s="10">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="10">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="10">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="10">
+        <v>10</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="10">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="10">
+        <v>11</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="10">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="10">
+        <v>12</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="10">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="10">
+        <v>13</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="10">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+      <c r="A15" s="10">
+        <v>14</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="10">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="10">
+        <v>15</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="10">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="10">
+        <v>16</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="10">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="10">
+        <v>17</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="14">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="10">
+        <v>18</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="14">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="10">
         <v>19</v>
       </c>
-      <c r="C7">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8">
+      <c r="C20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="10">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="10">
+        <v>20</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="10">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="10">
+        <v>21</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="10">
+        <v>1985</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="10">
+        <v>22</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="10">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="10">
+        <v>23</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="10">
+        <v>1998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="10">
+        <v>24</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="10">
+        <v>25</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="10">
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="10">
+        <v>26</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="10">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="10">
+        <v>27</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="10">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="10">
+        <v>28</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="10">
         <v>2007</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10">
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12">
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.35">
-      <c r="B14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16">
-        <v>2007</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="3">
-        <v>2007</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B18" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="3">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19">
-        <v>2010</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20">
-        <v>2005</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21">
-        <v>1985</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22">
-        <v>2004</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23">
-        <v>1998</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25">
-        <v>1997</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26">
-        <v>2003</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27">
-        <v>2004</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28">
-        <v>2007</v>
-      </c>
-    </row>
+    <row r="30" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>